<commit_message>
MOD Form: Validaciones doble email +  resumen comp
</commit_message>
<xml_diff>
--- a/src/data/listaProductos.xlsx
+++ b/src/data/listaProductos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material POSTGRADOS\CODERHOUSE\3. ReactJS (16955)\DESAFIOS\mitienda\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material POSTGRADOS\CODERHOUSE\3. ReactJS (16955)\DESAFIOS\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48E25BD-A864-4ECF-A896-9254C4A2781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494DAC60-285D-4FEE-BBC9-DB1E1CA9AA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17920" yWindow="4893" windowWidth="19200" windowHeight="10074" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
   </bookViews>
   <sheets>
     <sheet name="listaProductos" sheetId="2" r:id="rId1"/>
@@ -532,10 +532,10 @@
     <t>title</t>
   </si>
   <si>
-    <t>IdClasficacion</t>
-  </si>
-  <si>
     <t>descripcion</t>
+  </si>
+  <si>
+    <t>IdClasificacion</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
       <calculatedColumnFormula>RANDBETWEEN(5,20)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{ED895BA0-B7B4-4E9B-A22A-57C03807BB1D}" uniqueName="9" name="pictureUrl" queryTableFieldId="20"/>
-    <tableColumn id="10" xr3:uid="{2AE39C54-CC78-4ACE-9D94-D7F91CE2EB4C}" uniqueName="10" name="IdClasficacion" queryTableFieldId="22" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{2AE39C54-CC78-4ACE-9D94-D7F91CE2EB4C}" uniqueName="10" name="IdClasificacion" queryTableFieldId="22" dataDxfId="2">
       <calculatedColumnFormula>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{B813C5D0-C344-4D14-A4CD-500F272D5A2B}" uniqueName="12" name="IdGenero" queryTableFieldId="23" dataDxfId="1">
@@ -965,7 +965,7 @@
   <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1023,13 +1023,13 @@
         <v>80</v>
       </c>
       <c r="K1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L1" t="s">
         <v>79</v>
       </c>
       <c r="M1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I33" ca="1" si="0">RANDBETWEEN(5,20)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>81</v>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
         <v>82</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
         <v>83</v>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
         <v>84</v>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
         <v>85</v>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
         <v>86</v>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
         <v>87</v>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="J9" t="s">
         <v>88</v>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
         <v>89</v>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J11" t="s">
         <v>90</v>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J12" t="s">
         <v>91</v>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J13" t="s">
         <v>92</v>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J14" t="s">
         <v>93</v>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J15" t="s">
         <v>94</v>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J16" t="s">
         <v>95</v>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J17" t="s">
         <v>96</v>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J18" t="s">
         <v>97</v>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s">
         <v>98</v>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J20" t="s">
         <v>99</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J21" t="s">
         <v>100</v>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J22" t="s">
         <v>101</v>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J23" t="s">
         <v>102</v>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J24" t="s">
         <v>103</v>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J25" t="s">
         <v>104</v>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J27" t="s">
         <v>106</v>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J29" t="s">
         <v>108</v>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J30" t="s">
         <v>109</v>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J31" t="s">
         <v>110</v>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J32" t="s">
         <v>111</v>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J33" t="s">
         <v>112</v>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="I34">
         <f t="shared" ref="I34:I65" ca="1" si="1">RANDBETWEEN(5,20)</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J34" t="s">
         <v>113</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J35" t="s">
         <v>114</v>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J36" t="s">
         <v>115</v>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J37" t="s">
         <v>116</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J38" t="s">
         <v>117</v>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J39" t="s">
         <v>118</v>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J40" t="s">
         <v>119</v>
@@ -2814,7 +2814,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="J41" t="s">
         <v>120</v>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J42" t="s">
         <v>121</v>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J43" t="s">
         <v>122</v>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J44" t="s">
         <v>123</v>
@@ -2994,7 +2994,7 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J45" t="s">
         <v>124</v>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J46" t="s">
         <v>125</v>
@@ -3084,7 +3084,7 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J47" t="s">
         <v>126</v>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J48" t="s">
         <v>127</v>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J49" t="s">
         <v>128</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J51" t="s">
         <v>130</v>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J52" t="s">
         <v>131</v>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J53" t="s">
         <v>132</v>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J54" t="s">
         <v>133</v>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J55" t="s">
         <v>134</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J56" t="s">
         <v>135</v>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J57" t="s">
         <v>136</v>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J58" t="s">
         <v>137</v>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J59" t="s">
         <v>138</v>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J60" t="s">
         <v>139</v>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J61" t="s">
         <v>140</v>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J62" t="s">
         <v>141</v>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J63" t="s">
         <v>142</v>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J64" t="s">
         <v>143</v>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J65" t="s">
         <v>144</v>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I80" ca="1" si="2">RANDBETWEEN(5,20)</f>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J66" t="s">
         <v>145</v>
@@ -3984,7 +3984,7 @@
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J67" t="s">
         <v>146</v>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J68" t="s">
         <v>147</v>
@@ -4074,7 +4074,7 @@
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J69" t="s">
         <v>148</v>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J70" t="s">
         <v>149</v>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J71" t="s">
         <v>150</v>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J72" t="s">
         <v>151</v>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J73" t="s">
         <v>152</v>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="J74" t="s">
         <v>153</v>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J75" t="s">
         <v>154</v>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J76" t="s">
         <v>155</v>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J77" t="s">
         <v>156</v>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J78" t="s">
         <v>157</v>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J79" t="s">
         <v>158</v>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J80" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
reemplazo id x id_interno
</commit_message>
<xml_diff>
--- a/src/data/listaProductos.xlsx
+++ b/src/data/listaProductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material POSTGRADOS\CODERHOUSE\3. ReactJS (16955)\DESAFIOS\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494DAC60-285D-4FEE-BBC9-DB1E1CA9AA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE9E0FD-2530-4BDB-801E-8B5B5ABC9B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>under-armour</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>clasificacion</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
   </si>
   <si>
     <t>IdClasificacion</t>
+  </si>
+  <si>
+    <t>id_interno</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA90D056-4F86-4DE6-9183-BAEC54425CE0}" name="listaProductos" displayName="listaProductos" ref="A1:M80" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:M80" xr:uid="{BA90D056-4F86-4DE6-9183-BAEC54425CE0}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{F0AEF119-BE71-483B-8F4E-EAEE36A96068}" uniqueName="1" name="id" queryTableFieldId="12" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{F0AEF119-BE71-483B-8F4E-EAEE36A96068}" uniqueName="1" name="id_interno" queryTableFieldId="12" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{7CCF6AEC-57B0-44B2-B173-C7FA7C1B08FB}" uniqueName="2" name="clasificacion" queryTableFieldId="13"/>
     <tableColumn id="3" xr3:uid="{3604E10F-B460-4B30-A009-FB559EDCB777}" uniqueName="3" name="tipo" queryTableFieldId="14"/>
     <tableColumn id="4" xr3:uid="{031384C2-8068-46E8-8C75-3BF309952241}" uniqueName="4" name="title" queryTableFieldId="15"/>
@@ -965,7 +965,7 @@
   <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -993,43 +993,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
         <v>161</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">
@@ -1059,10 +1059,10 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I33" ca="1" si="0">RANDBETWEEN(5,20)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1104,10 +1104,10 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K3">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1149,10 +1149,10 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1197,7 +1197,7 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1239,10 +1239,10 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1284,10 +1284,10 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K7">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1329,10 +1329,10 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K8">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1374,10 +1374,10 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1419,10 +1419,10 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K10">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1464,10 +1464,10 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K11">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1509,10 +1509,10 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K12">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1554,10 +1554,10 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K13">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1599,10 +1599,10 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K14">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1644,10 +1644,10 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K15">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1689,10 +1689,10 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K16">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1734,10 +1734,10 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K17">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1779,10 +1779,10 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K18">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1824,10 +1824,10 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K19">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1869,10 +1869,10 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K20">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1914,10 +1914,10 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -1959,10 +1959,10 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K22">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2004,10 +2004,10 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K23">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2049,10 +2049,10 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K24">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2094,10 +2094,10 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K25">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2139,10 +2139,10 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K26">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2184,10 +2184,10 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K27">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2229,10 +2229,10 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K28">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2274,10 +2274,10 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K29">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2319,10 +2319,10 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K30">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2364,10 +2364,10 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K31">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2409,10 +2409,10 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K32">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2454,10 +2454,10 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K33">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2499,10 +2499,10 @@
       </c>
       <c r="I34">
         <f t="shared" ref="I34:I65" ca="1" si="1">RANDBETWEEN(5,20)</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K34">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2544,10 +2544,10 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K35">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2589,10 +2589,10 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K36">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2634,10 +2634,10 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K37">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2679,10 +2679,10 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K38">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2724,10 +2724,10 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K39">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2769,10 +2769,10 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K40">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2814,10 +2814,10 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K41">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2859,10 +2859,10 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K42">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2904,10 +2904,10 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K43">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2949,10 +2949,10 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K44">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -2994,10 +2994,10 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K45">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3039,10 +3039,10 @@
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K46">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3084,10 +3084,10 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K47">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3129,10 +3129,10 @@
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K48">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3174,10 +3174,10 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K49">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3219,10 +3219,10 @@
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K50">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3267,7 +3267,7 @@
         <v>9</v>
       </c>
       <c r="J51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K51">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3309,10 +3309,10 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K52">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3354,10 +3354,10 @@
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K53">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3399,10 +3399,10 @@
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K54">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3444,10 +3444,10 @@
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K55">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3489,10 +3489,10 @@
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K56">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3534,10 +3534,10 @@
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K57">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3579,10 +3579,10 @@
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K58">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3624,10 +3624,10 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K59">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3669,10 +3669,10 @@
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K60">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3714,10 +3714,10 @@
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K61">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3759,10 +3759,10 @@
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K62">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3804,10 +3804,10 @@
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K63">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3849,10 +3849,10 @@
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K64">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3894,10 +3894,10 @@
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K65">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3942,7 +3942,7 @@
         <v>9</v>
       </c>
       <c r="J66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K66">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -3984,10 +3984,10 @@
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K67">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4029,10 +4029,10 @@
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K68">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4074,10 +4074,10 @@
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K69">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4119,10 +4119,10 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K70">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4164,10 +4164,10 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K71">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4209,10 +4209,10 @@
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K72">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4254,10 +4254,10 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K73">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4299,10 +4299,10 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K74">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4344,10 +4344,10 @@
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K75">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4389,10 +4389,10 @@
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K76">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4434,10 +4434,10 @@
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K77">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4479,10 +4479,10 @@
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K78">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4524,10 +4524,10 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K79">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
@@ -4569,10 +4569,10 @@
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K80">
         <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>

</xml_diff>

<commit_message>
modifico nombres atributos: category, IdCategory
</commit_message>
<xml_diff>
--- a/src/data/listaProductos.xlsx
+++ b/src/data/listaProductos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material POSTGRADOS\CODERHOUSE\3. ReactJS (16955)\DESAFIOS\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE9E0FD-2530-4BDB-801E-8B5B5ABC9B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E89768-D842-41EA-93F0-A6B9004D6269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10073" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
   </bookViews>
   <sheets>
     <sheet name="listaProductos" sheetId="2" r:id="rId1"/>
@@ -262,9 +262,6 @@
     <t>under-armour</t>
   </si>
   <si>
-    <t>clasificacion</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -532,10 +529,13 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>IdClasificacion</t>
-  </si>
-  <si>
     <t>id_interno</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>IdCategory</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <autoFilter ref="A1:M80" xr:uid="{BA90D056-4F86-4DE6-9183-BAEC54425CE0}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F0AEF119-BE71-483B-8F4E-EAEE36A96068}" uniqueName="1" name="id_interno" queryTableFieldId="12" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7CCF6AEC-57B0-44B2-B173-C7FA7C1B08FB}" uniqueName="2" name="clasificacion" queryTableFieldId="13"/>
+    <tableColumn id="2" xr3:uid="{7CCF6AEC-57B0-44B2-B173-C7FA7C1B08FB}" uniqueName="2" name="category" queryTableFieldId="13"/>
     <tableColumn id="3" xr3:uid="{3604E10F-B460-4B30-A009-FB559EDCB777}" uniqueName="3" name="tipo" queryTableFieldId="14"/>
     <tableColumn id="4" xr3:uid="{031384C2-8068-46E8-8C75-3BF309952241}" uniqueName="4" name="title" queryTableFieldId="15"/>
     <tableColumn id="5" xr3:uid="{1842771E-5F67-4881-93E7-0CD13AC29E7D}" uniqueName="5" name="marca" queryTableFieldId="16"/>
@@ -651,8 +651,8 @@
       <calculatedColumnFormula>RANDBETWEEN(5,20)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{ED895BA0-B7B4-4E9B-A22A-57C03807BB1D}" uniqueName="9" name="pictureUrl" queryTableFieldId="20"/>
-    <tableColumn id="10" xr3:uid="{2AE39C54-CC78-4ACE-9D94-D7F91CE2EB4C}" uniqueName="10" name="IdClasificacion" queryTableFieldId="22" dataDxfId="2">
-      <calculatedColumnFormula>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{2AE39C54-CC78-4ACE-9D94-D7F91CE2EB4C}" uniqueName="10" name="IdCategory" queryTableFieldId="22" dataDxfId="2">
+      <calculatedColumnFormula>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{B813C5D0-C344-4D14-A4CD-500F272D5A2B}" uniqueName="12" name="IdGenero" queryTableFieldId="23" dataDxfId="1">
       <calculatedColumnFormula>IF(listaProductos[[#This Row],[genero]]="mujer",1,IF(listaProductos[[#This Row],[genero]]="hombre",2,IF(listaProductos[[#This Row],[genero]]="unisex",3,IF(listaProductos[[#This Row],[genero]]="nino",4))))</calculatedColumnFormula>
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3A9513-E27C-4A89-9A7E-C5AED3C3978D}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -993,43 +993,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" t="s">
         <v>160</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">
@@ -1059,13 +1059,13 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I33" ca="1" si="0">RANDBETWEEN(5,20)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L2">
@@ -1104,13 +1104,13 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L3">
@@ -1149,13 +1149,13 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L4">
@@ -1194,13 +1194,13 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L5">
@@ -1239,13 +1239,13 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L6">
@@ -1284,13 +1284,13 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L7">
@@ -1329,13 +1329,13 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K8">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L8">
@@ -1374,13 +1374,13 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K9">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L9">
@@ -1419,13 +1419,13 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K10">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L10">
@@ -1464,13 +1464,13 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L11">
@@ -1509,13 +1509,13 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K12">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L12">
@@ -1554,13 +1554,13 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K13">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L13">
@@ -1599,13 +1599,13 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K14">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>1</v>
       </c>
       <c r="L14">
@@ -1644,13 +1644,13 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K15">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L15">
@@ -1689,13 +1689,13 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K16">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L16">
@@ -1734,13 +1734,13 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K17">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L17">
@@ -1779,13 +1779,13 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K18">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L18">
@@ -1824,13 +1824,13 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K19">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L19">
@@ -1869,13 +1869,13 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K20">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L20">
@@ -1914,13 +1914,13 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K21">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L21">
@@ -1959,13 +1959,13 @@
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K22">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L22">
@@ -2004,13 +2004,13 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K23">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L23">
@@ -2049,13 +2049,13 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K24">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L24">
@@ -2094,13 +2094,13 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K25">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L25">
@@ -2139,13 +2139,13 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K26">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L26">
@@ -2184,13 +2184,13 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K27">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L27">
@@ -2229,13 +2229,13 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K28">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L28">
@@ -2277,10 +2277,10 @@
         <v>19</v>
       </c>
       <c r="J29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K29">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L29">
@@ -2319,13 +2319,13 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K30">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L30">
@@ -2364,13 +2364,13 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K31">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L31">
@@ -2409,13 +2409,13 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K32">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L32">
@@ -2454,13 +2454,13 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K33">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L33">
@@ -2499,13 +2499,13 @@
       </c>
       <c r="I34">
         <f t="shared" ref="I34:I65" ca="1" si="1">RANDBETWEEN(5,20)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K34">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L34">
@@ -2544,13 +2544,13 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K35">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L35">
@@ -2589,13 +2589,13 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K36">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L36">
@@ -2634,13 +2634,13 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K37">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L37">
@@ -2679,13 +2679,13 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K38">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L38">
@@ -2724,13 +2724,13 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K39">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L39">
@@ -2769,13 +2769,13 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K40">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L40">
@@ -2814,13 +2814,13 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K41">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L41">
@@ -2859,13 +2859,13 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K42">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L42">
@@ -2904,13 +2904,13 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K43">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L43">
@@ -2949,13 +2949,13 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K44">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L44">
@@ -2994,13 +2994,13 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K45">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L45">
@@ -3039,13 +3039,13 @@
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K46">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>2</v>
       </c>
       <c r="L46">
@@ -3084,13 +3084,13 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K47">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L47">
@@ -3129,13 +3129,13 @@
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K48">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L48">
@@ -3174,13 +3174,13 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K49">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L49">
@@ -3222,10 +3222,10 @@
         <v>5</v>
       </c>
       <c r="J50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K50">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L50">
@@ -3264,13 +3264,13 @@
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K51">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L51">
@@ -3309,13 +3309,13 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="J52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K52">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L52">
@@ -3354,13 +3354,13 @@
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K53">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L53">
@@ -3399,13 +3399,13 @@
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K54">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L54">
@@ -3444,13 +3444,13 @@
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K55">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L55">
@@ -3489,13 +3489,13 @@
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K56">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L56">
@@ -3534,13 +3534,13 @@
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K57">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L57">
@@ -3579,13 +3579,13 @@
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K58">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L58">
@@ -3624,13 +3624,13 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K59">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L59">
@@ -3669,13 +3669,13 @@
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="J60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K60">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L60">
@@ -3714,13 +3714,13 @@
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K61">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L61">
@@ -3759,13 +3759,13 @@
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K62">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L62">
@@ -3804,13 +3804,13 @@
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K63">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L63">
@@ -3849,13 +3849,13 @@
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K64">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L64">
@@ -3894,13 +3894,13 @@
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K65">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L65">
@@ -3939,13 +3939,13 @@
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I80" ca="1" si="2">RANDBETWEEN(5,20)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K66">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L66">
@@ -3984,13 +3984,13 @@
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="J67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K67">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L67">
@@ -4029,13 +4029,13 @@
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K68">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L68">
@@ -4074,13 +4074,13 @@
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K69">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L69">
@@ -4119,13 +4119,13 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K70">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L70">
@@ -4164,13 +4164,13 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K71">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L71">
@@ -4209,13 +4209,13 @@
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="J72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K72">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L72">
@@ -4254,13 +4254,13 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K73">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L73">
@@ -4299,13 +4299,13 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K74">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L74">
@@ -4344,13 +4344,13 @@
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K75">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L75">
@@ -4389,13 +4389,13 @@
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K76">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L76">
@@ -4434,13 +4434,13 @@
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J77" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K77">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L77">
@@ -4479,13 +4479,13 @@
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K78">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L78">
@@ -4524,13 +4524,13 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K79">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L79">
@@ -4569,13 +4569,13 @@
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K80">
-        <f>IF(listaProductos[[#This Row],[clasificacion]]="accesorio",1,IF(listaProductos[[#This Row],[clasificacion]]="calzado",2,IF(listaProductos[[#This Row],[clasificacion]]="vestir",3)))</f>
+        <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
         <v>3</v>
       </c>
       <c r="L80">

</xml_diff>

<commit_message>
Cambio url img lista productos firebase
</commit_message>
<xml_diff>
--- a/src/data/listaProductos.xlsx
+++ b/src/data/listaProductos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material POSTGRADOS\CODERHOUSE\3. ReactJS (16955)\DESAFIOS\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E89768-D842-41EA-93F0-A6B9004D6269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E643CF9C-B884-4025-9B08-F31FF51A0687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10073" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{3C1A2436-EC64-48AE-97CC-C4597AA4688F}"/>
   </bookViews>
   <sheets>
     <sheet name="listaProductos" sheetId="2" r:id="rId1"/>
@@ -283,243 +283,6 @@
     <t>pictureUrl</t>
   </si>
   <si>
-    <t>images/accesorio_casual_billetera_tommy-hilfiger_hombre_negro_cuero.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_casual_gafas_timberland_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_casual_reloj_tommy-hilfiger_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_casual_reloj_tommy-hilfiger_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_casual_reloj-pro_tommy-hilfiger_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_balon_nike_unisex_verde.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_gafas_oakley_hombre_negro_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_gafas_oakley_hombre_negro_naranja.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_gorra_nike_hombre_blanco.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_gorra_oakley_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_deporte_gorra_oakley_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_trekking_bandana_the-north-face_hombre_rojo.jpg</t>
-  </si>
-  <si>
-    <t>images/accesorio_trekking_gorro_the-north-face_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_botas_timberland_mujer_cafe.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_botas_timberland_mujer_marron.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_botas_timberland_nino_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_sandalia_timberland_mujer_cafe.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_sandalia_timberland_mujer_miel.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_sandalia_timberland_mujer_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_sandalia_timberland_mujer_rojo.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_sandalia_tommy-hilfiger_mujer_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_nike_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_polo-ralph-lauren_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_puma_mujer_blanco.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_hombre_azul_cafe.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_hombre_azul_slim.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_hombre_olivo.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_timberland_mujer_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_tommy-hilfiger_mujer_blanco.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_casual_tenis_tommy-hilfiger_mujer_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_botin_nike_hombre_salmon.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_tenis_nike_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_tenis_nike_mujer_rosado.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_tenis_puma_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_tenis_puma_mujer_rosado.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_deporte_tenis_skechers_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_informal_playera_nautica_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_informal_playera_nautica_hombre_rojo.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_informal_playera_puma_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_informal_playera_the-north-face_mujer_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_informal_playera-slim_nautica_hombre_rojo.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_trabajo_bota_timberland_hombre_cafe.jpg</t>
-  </si>
-  <si>
-    <t>images/calzado_trekking_bota_the-north-face_hombre_cafe.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_camisa_polo-ralph-lauren_hombre_azul_rayas.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_camisa_polo-ralph-lauren_hombre_olivo.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_camisa_polo-ralph-lauren_hombre_salmon.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_camisa_polo-ralph-lauren_hombre_verde_cuadros.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_chaqueta_polo-ralph-lauren_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_chaqueta_polo-ralph-lauren_hombre_rojo.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_chaqueta_the-north-face_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_chaqueta_the-north-face_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_pantalon_polo-ralph-lauren_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_pantalon_polo-ralph-lauren_hombre_caqui.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_pantalon_polo-ralph-lauren_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_pantalon_polo-ralph-lauren_hombre_olivo.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_calvin-klein_hombre_navy.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_calvin-klein_mujer_salmon.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_frida-kahlo_mujer_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_gap_hombre_navy.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_gap_hombre_negra.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_gap_unisex_verde.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_harry-potter_mujer_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_levis_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_nickelodeon_mujer_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_nike_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_reebok_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_reebok_mujer_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_remera_snoopy_nina_coral.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_saco_polo-ralph-lauren_hombre_beige.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_sweater-hoodie_polo-ralph-lauren_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_casual_sweater-hoodie_the-north-face_mujer_rosado.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_chaqueta_nike_hombre_azul.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_conjunto-ciclismo_xtiger_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_polo_nike_hombre_negro.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_remera_adidas_hombre_blanco.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_remera_nike_hombre_gris.jpg</t>
-  </si>
-  <si>
-    <t>images/vestir_deporte_remera_under-armour_hombre_azul.jpg</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -536,6 +299,243 @@
   </si>
   <si>
     <t>IdCategory</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_casual_billetera_tommy-hilfiger_hombre_negro_cuero.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_casual_gafas_timberland_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_casual_reloj_tommy-hilfiger_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_casual_reloj_tommy-hilfiger_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_casual_reloj-pro_tommy-hilfiger_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_balon_nike_unisex_verde.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_gafas_oakley_hombre_negro_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_gafas_oakley_hombre_negro_naranja.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_gorra_nike_hombre_blanco.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_gorra_oakley_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_deporte_gorra_oakley_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_trekking_bandana_the-north-face_hombre_rojo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/accesorio_trekking_gorro_the-north-face_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_botas_timberland_mujer_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_botas_timberland_mujer_marron.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_botas_timberland_nino_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_sandalia_timberland_mujer_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_sandalia_timberland_mujer_miel.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_sandalia_timberland_mujer_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_sandalia_timberland_mujer_rojo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_sandalia_tommy-hilfiger_mujer_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_nike_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_polo-ralph-lauren_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_puma_mujer_blanco.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_hombre_azul_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_hombre_azul_slim.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_hombre_olivo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_timberland_mujer_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_tommy-hilfiger_mujer_blanco.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_casual_tenis_tommy-hilfiger_mujer_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_botin_nike_hombre_salmon.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_tenis_nike_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_tenis_nike_mujer_rosado.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_tenis_puma_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_tenis_puma_mujer_rosado.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_deporte_tenis_skechers_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_informal_playera_nautica_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_informal_playera_nautica_hombre_rojo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_informal_playera_puma_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_informal_playera_the-north-face_mujer_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_informal_playera-slim_nautica_hombre_rojo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_trabajo_bota_timberland_hombre_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/calzado_trekking_bota_the-north-face_hombre_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_camisa_polo-ralph-lauren_hombre_azul_rayas.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_camisa_polo-ralph-lauren_hombre_olivo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_camisa_polo-ralph-lauren_hombre_salmon.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_camisa_polo-ralph-lauren_hombre_verde_cuadros.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_chaqueta_polo-ralph-lauren_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_chaqueta_polo-ralph-lauren_hombre_rojo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_chaqueta_the-north-face_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_chaqueta_the-north-face_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_pantalon_polo-ralph-lauren_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_pantalon_polo-ralph-lauren_hombre_caqui.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_pantalon_polo-ralph-lauren_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_pantalon_polo-ralph-lauren_hombre_olivo.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_calvin-klein_hombre_navy.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_calvin-klein_mujer_salmon.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_frida-kahlo_mujer_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_gap_hombre_navy.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_gap_hombre_negra.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_gap_unisex_verde.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_harry-potter_mujer_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_levis_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_nickelodeon_mujer_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_nike_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_reebok_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_reebok_mujer_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_remera_snoopy_nina_coral.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_saco_polo-ralph-lauren_hombre_beige.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_sweater-hoodie_polo-ralph-lauren_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_casual_sweater-hoodie_the-north-face_mujer_rosado.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_chaqueta_nike_hombre_azul.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_conjunto-ciclismo_xtiger_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_polo_nike_hombre_negro.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_remera_adidas_hombre_blanco.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_remera_nike_hombre_gris.jpg</t>
+  </si>
+  <si>
+    <t>https://ecommerce-ab.web.app/images/vestir_deporte_remera_under-armour_hombre_azul.jpg</t>
   </si>
 </sst>
 </file>
@@ -965,7 +965,7 @@
   <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -993,16 +993,16 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
         <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
         <v>73</v>
@@ -1014,7 +1014,7 @@
         <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s">
         <v>76</v>
@@ -1023,13 +1023,13 @@
         <v>78</v>
       </c>
       <c r="K1" t="s">
-        <v>163</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>77</v>
       </c>
       <c r="M1" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.5">
@@ -1059,10 +1059,10 @@
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I33" ca="1" si="0">RANDBETWEEN(5,20)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K2">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1104,10 +1104,10 @@
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="K3">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1152,7 +1152,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="K4">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1194,10 +1194,10 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="K5">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1239,10 +1239,10 @@
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="K6">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1284,10 +1284,10 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K7">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1329,10 +1329,10 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="K8">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1374,10 +1374,10 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K9">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1419,10 +1419,10 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K10">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1464,10 +1464,10 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="K11">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1509,10 +1509,10 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K12">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1554,10 +1554,10 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K13">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1599,10 +1599,10 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J14" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="K14">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1644,10 +1644,10 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J15" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K15">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1689,10 +1689,10 @@
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="K16">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1734,10 +1734,10 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="K17">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1779,10 +1779,10 @@
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="K18">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1824,10 +1824,10 @@
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="K19">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1869,10 +1869,10 @@
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J20" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K20">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1914,10 +1914,10 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="K21">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -1962,7 +1962,7 @@
         <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="K22">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2004,10 +2004,10 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="K23">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2049,10 +2049,10 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="K24">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2094,10 +2094,10 @@
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J25" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="K25">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2139,10 +2139,10 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="K26">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2184,10 +2184,10 @@
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K27">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2229,10 +2229,10 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K28">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2274,10 +2274,10 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="K29">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2319,10 +2319,10 @@
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J30" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="K30">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2364,10 +2364,10 @@
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J31" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K31">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2409,10 +2409,10 @@
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="K32">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2454,10 +2454,10 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="K33">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2499,10 +2499,10 @@
       </c>
       <c r="I34">
         <f t="shared" ref="I34:I65" ca="1" si="1">RANDBETWEEN(5,20)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J34" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="K34">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2544,10 +2544,10 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J35" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="K35">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2589,10 +2589,10 @@
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J36" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="K36">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2634,10 +2634,10 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J37" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="K37">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2679,10 +2679,10 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J38" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K38">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2724,10 +2724,10 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J39" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="K39">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2769,10 +2769,10 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="K40">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2814,10 +2814,10 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J41" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="K41">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2859,10 +2859,10 @@
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J42" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="K42">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2904,10 +2904,10 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J43" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="K43">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2949,10 +2949,10 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="K44">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -2994,10 +2994,10 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J45" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="K45">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3039,10 +3039,10 @@
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J46" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="K46">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3084,10 +3084,10 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J47" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K47">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3129,10 +3129,10 @@
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J48" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="K48">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3174,10 +3174,10 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="K49">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3219,10 +3219,10 @@
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="J50" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="K50">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3267,7 +3267,7 @@
         <v>14</v>
       </c>
       <c r="J51" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="K51">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3309,10 +3309,10 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J52" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="K52">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3354,10 +3354,10 @@
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J53" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K53">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3399,10 +3399,10 @@
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J54" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="K54">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3444,10 +3444,10 @@
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J55" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="K55">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3489,10 +3489,10 @@
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J56" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K56">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3537,7 +3537,7 @@
         <v>9</v>
       </c>
       <c r="J57" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="K57">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3579,10 +3579,10 @@
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J58" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="K58">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3624,10 +3624,10 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J59" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K59">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3669,10 +3669,10 @@
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="J60" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="K60">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3714,10 +3714,10 @@
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J61" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="K61">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3759,10 +3759,10 @@
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J62" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K62">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3804,10 +3804,10 @@
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J63" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="K63">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3852,7 +3852,7 @@
         <v>18</v>
       </c>
       <c r="J64" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="K64">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3894,10 +3894,10 @@
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J65" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K65">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3939,10 +3939,10 @@
       </c>
       <c r="I66">
         <f t="shared" ref="I66:I80" ca="1" si="2">RANDBETWEEN(5,20)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J66" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K66">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -3984,10 +3984,10 @@
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="K67">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4029,10 +4029,10 @@
       </c>
       <c r="I68">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J68" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="K68">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4074,10 +4074,10 @@
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J69" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="K69">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4119,10 +4119,10 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J70" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="K70">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4164,10 +4164,10 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J71" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="K71">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4209,10 +4209,10 @@
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J72" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="K72">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4254,10 +4254,10 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J73" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="K73">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4299,10 +4299,10 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="J74" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="K74">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4344,10 +4344,10 @@
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="J75" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="K75">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4389,10 +4389,10 @@
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J76" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="K76">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4434,10 +4434,10 @@
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J77" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="K77">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4479,10 +4479,10 @@
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J78" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="K78">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4524,10 +4524,10 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J79" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K79">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>
@@ -4569,10 +4569,10 @@
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J80" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="K80">
         <f>IF(listaProductos[[#This Row],[category]]="accesorio",1,IF(listaProductos[[#This Row],[category]]="calzado",2,IF(listaProductos[[#This Row],[category]]="vestir",3)))</f>

</xml_diff>